<commit_message>
updated some work 3.16
</commit_message>
<xml_diff>
--- a/SALT/SALT_properties.xlsx
+++ b/SALT/SALT_properties.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beelbw/Documents/LDRD_FY20_SALT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natiben/myrepo/spreadsheets/SALT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C71CEB-9BE6-C44B-85F2-81626450DF54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDEAC9E-17A0-3845-8BF5-0B06A95FAF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{1438BF92-828F-7149-A6D5-4B22AB4873A7}"/>
+    <workbookView xWindow="1000" yWindow="3480" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{1438BF92-828F-7149-A6D5-4B22AB4873A7}"/>
   </bookViews>
   <sheets>
     <sheet name="KCl" sheetId="1" r:id="rId1"/>
     <sheet name="LiCl_80KCl" sheetId="2" r:id="rId2"/>
     <sheet name="NaCl_MgCl2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>KCl equilibrations</t>
   </si>
@@ -45,6 +51,9 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>LiCl-80KCl equilibrations</t>
   </si>
 </sst>
 </file>
@@ -148,10 +157,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>KCl!$G$6:$G$10</c:f>
+              <c:f>KCl!$G$6:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6518.04</c:v>
                 </c:pt>
@@ -166,16 +175,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8675.5112399999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9280.5686718750003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9913.1240849999976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>KCl!$F$6:$F$10</c:f>
+              <c:f>KCl!$F$6:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>19.802406666666698</c:v>
                 </c:pt>
@@ -185,8 +200,17 @@
                 <c:pt idx="2">
                   <c:v>5.9041266666666701</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6969799999999999</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>-9.4726666666666695E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.80862000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.81626</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -195,6 +219,79 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2414-364F-8BDB-030FFEE06D75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>KCl!$G$15:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6859.28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7415.1776920833954</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000.3265782184035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8615.476689021727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9261.378055110079</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>KCl!$F$15:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.896513333333299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2037000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6605-9142-812F-0EF2D0A841FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -213,6 +310,8 @@
         <c:axId val="1014847472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+          <c:min val="6000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1742,8 +1841,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2112,7 +2211,7 @@
   <dimension ref="B3:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B3" sqref="B3:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2170,7 +2269,7 @@
         <v>5.9041266666666701</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="0">G7*((D8/D7)^(3))</f>
+        <f t="shared" ref="G8:G12" si="0">G7*((D8/D7)^(3))</f>
         <v>7545.4460549999994</v>
       </c>
     </row>
@@ -2178,6 +2277,12 @@
       <c r="D9">
         <v>1.075</v>
       </c>
+      <c r="E9">
+        <v>-631.34152687333403</v>
+      </c>
+      <c r="F9">
+        <v>2.6969799999999999</v>
+      </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>8097.3407231249976</v>
@@ -2202,11 +2307,31 @@
       <c r="D11">
         <v>1.125</v>
       </c>
+      <c r="E11">
+        <v>-626.46267805333298</v>
+      </c>
+      <c r="F11">
+        <v>-0.80862000000000001</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>9280.5686718750003</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>1.1499999999999999</v>
       </c>
+      <c r="E12">
+        <v>-623.38357945333303</v>
+      </c>
+      <c r="F12">
+        <v>-1.81626</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>9913.1240849999976</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D14">
@@ -2217,78 +2342,109 @@
       <c r="D15">
         <v>0.95</v>
       </c>
+      <c r="E15">
+        <v>-635.36910887999898</v>
+      </c>
+      <c r="F15">
+        <v>12.896513333333299</v>
+      </c>
+      <c r="G15">
+        <v>6859.28</v>
+      </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>0.97499999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>-635.38609069999995</v>
+      </c>
+      <c r="F16">
+        <v>6.2037000000000004</v>
+      </c>
+      <c r="G16">
+        <f>G15*((D16/D15)^(3))</f>
+        <v>7415.1776920833954</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f t="shared" ref="G17:G19" si="1">G16*((D17/D16)^(3))</f>
+        <v>8000.3265782184035</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>1.0249999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>8615.476689021727</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>9261.378055110079</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>800</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>0.95</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D26">
         <v>1.05</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D28">
         <v>700</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D29">
         <v>0.95</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D32">
         <v>1.0249999999999999</v>
       </c>
@@ -2306,22 +2462,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42FAA31-0BF7-0A47-A1FF-DA8766D4C63C}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0.95</v>
+      </c>
+      <c r="E5">
+        <v>-645.49680606666595</v>
+      </c>
+      <c r="F5">
+        <v>35.19162</v>
+      </c>
+      <c r="G5">
+        <v>5588.41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G6">
+        <f>G5*((D6/D5)^(3))</f>
+        <v>6041.3123777154115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>-648.61861583333302</v>
+      </c>
+      <c r="F7">
+        <v>14.8488133333333</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G13" si="0">G6*((D7/D6)^(3))</f>
+        <v>6518.0463624435088</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="E8">
+        <v>-648.88683186666697</v>
+      </c>
+      <c r="F8">
+        <v>8.2293666666666692</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>7019.2230210307662</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1.05</v>
+      </c>
+      <c r="E9">
+        <v>-646.176745193334</v>
+      </c>
+      <c r="F9">
+        <v>4.9316599999999999</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>7545.4534203236663</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>1.075</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>8097.3486271686861</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>8675.5197084123101</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>1.125</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>9280.5777309010118</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>9913.1337614812692</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0386EE-94F0-D14A-AAF9-31FA05A213F8}">
-  <dimension ref="B4:F10"/>
+  <dimension ref="B4:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2419,6 +2692,75 @@
         <v>8823.2931943432031</v>
       </c>
     </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>0.9</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F16" si="1">F15*(C14/C15)^3</f>
+        <v>5556.3547483095408</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>0.95</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>6534.8143379038293</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>7621.8858001502613</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>1.05</v>
+      </c>
+      <c r="F17">
+        <f>F18*(C17/C18)^3</f>
+        <v>8823.2855493989464</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D18">
+        <v>-639.56252220666704</v>
+      </c>
+      <c r="E18">
+        <v>-2.83110666666667</v>
+      </c>
+      <c r="F18">
+        <v>10144.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>